<commit_message>
Edit offerte G24 + Complete voorstelling g24
</commit_message>
<xml_diff>
--- a/opdracht03/documentatie/Offerte groep 24.xlsx
+++ b/opdracht03/documentatie/Offerte groep 24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2\Vakken\Projecten 2\p2ops-g10\opdracht03\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8B8AE2-F13A-4C39-A860-5CC05B1CDA66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08065E90-CAFF-4CFD-8B98-79AE9A609AB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Offerte</t>
   </si>
@@ -117,18 +117,12 @@
     <t>Epson EH-TW650 - Full HD 3LCD - Wi-Fi Beamer</t>
   </si>
   <si>
-    <t>Elite Screens M120XWH2 (16:9) 273 x 167 - Projectiescherm</t>
-  </si>
-  <si>
     <t>Vogel's VPC 545 - Beugel voor beamer</t>
   </si>
   <si>
     <t>Ricoh MPC 2003SP-G - Kopieermachine &amp; Printer</t>
   </si>
   <si>
-    <t>Htek UC924 4-Line Gigabit - IP Phone</t>
-  </si>
-  <si>
     <t>Nikon D3500 - Fotocamera</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>AutoCAD Licentie - 1 jaar</t>
   </si>
   <si>
-    <t>Microsoft Office 365 - 1 jaar</t>
-  </si>
-  <si>
     <t>Installatie</t>
   </si>
   <si>
@@ -190,6 +181,24 @@
   </si>
   <si>
     <t>Hardware</t>
+  </si>
+  <si>
+    <t>Elite Screens M92XWH (16:9) 212 x 140 - Projectiescherm</t>
+  </si>
+  <si>
+    <t>HDMI kabel 1 meter</t>
+  </si>
+  <si>
+    <t>HDMI kabel 5 meter</t>
+  </si>
+  <si>
+    <t>Microsoft Office 365 Business Premium - 1 jaar</t>
+  </si>
+  <si>
+    <t>Htek UC924 4-Line Gigabit - VoIP Telefoon</t>
+  </si>
+  <si>
+    <t>TP-Link DOCSIS 3.0 Modem</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -469,11 +478,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -564,101 +604,148 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="11.35" x14ac:dyDescent="0.35"/>
@@ -1035,10 +1122,10 @@
       <c r="C3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="53"/>
+      <c r="D3" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="66"/>
       <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
@@ -1053,10 +1140,10 @@
       <c r="C4" s="37">
         <v>43603</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="55"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="38" t="s">
         <v>11</v>
       </c>
@@ -1070,10 +1157,10 @@
       <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1088,10 +1175,10 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="48"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
@@ -1106,10 +1193,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="43"/>
+      <c r="A9" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="70"/>
       <c r="C9" s="5">
         <v>1</v>
       </c>
@@ -1120,15 +1207,15 @@
         <v>0.21</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" ref="F9:F15" si="0">SUM(C9*D9)</f>
+        <f t="shared" ref="F9:F16" si="0">SUM(C9*D9)</f>
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="43"/>
+      <c r="A10" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="70"/>
       <c r="C10" s="5">
         <v>1</v>
       </c>
@@ -1144,10 +1231,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="43"/>
+      <c r="A11" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="70"/>
       <c r="C11" s="5">
         <v>1</v>
       </c>
@@ -1162,823 +1249,883 @@
         <v>118.2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="43"/>
+    <row r="12" spans="1:6" s="63" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="70"/>
       <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="6">
+        <v>44.6</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F12" s="8">
+        <f>SUM(C12*D12)</f>
+        <v>44.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="70"/>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6">
         <v>119</v>
       </c>
-      <c r="E12" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E13" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="5">
+    <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D14" s="6">
         <v>1.36</v>
       </c>
-      <c r="E13" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E14" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="5">
+    <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="70"/>
+      <c r="C15" s="5">
         <v>3</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D15" s="6">
         <v>1.42</v>
       </c>
-      <c r="E14" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E15" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F15" s="8">
         <f t="shared" si="0"/>
         <v>4.26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="31">
+    <row r="16" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="80" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="81"/>
+      <c r="C16" s="31">
         <v>5</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D16" s="32">
         <v>5.04</v>
       </c>
-      <c r="E15" s="33">
-        <v>0.21</v>
-      </c>
-      <c r="F15" s="34">
+      <c r="E16" s="33">
+        <v>0.21</v>
+      </c>
+      <c r="F16" s="34">
         <f t="shared" si="0"/>
         <v>25.2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="47"/>
+    <row r="17" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="30"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="25"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="48" t="s">
+    <row r="18" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="72"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="41" t="s">
+      <c r="B20" s="73"/>
+      <c r="C20" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F20" s="41" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="66">
+    <row r="21" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="88"/>
+      <c r="C21" s="57">
         <v>16</v>
       </c>
-      <c r="D20" s="67">
+      <c r="D21" s="58">
         <v>62</v>
       </c>
-      <c r="E20" s="68">
-        <v>0.21</v>
-      </c>
-      <c r="F20" s="69">
-        <f>SUM(C20*D20)</f>
+      <c r="E21" s="59">
+        <v>0.21</v>
+      </c>
+      <c r="F21" s="60">
+        <f>SUM(C21*D21)</f>
         <v>992</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="25"/>
-    </row>
     <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="60"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="25"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="56"/>
     </row>
     <row r="23" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="63"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="25"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="71"/>
       <c r="C24" s="24"/>
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
       <c r="F24" s="25"/>
     </row>
-    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
+    <row r="25" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
       <c r="F25" s="25"/>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
       <c r="D26" s="12"/>
       <c r="E26" s="13"/>
       <c r="F26" s="25"/>
     </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="48" t="s">
+    <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="21" t="s">
+      <c r="B28" s="73"/>
+      <c r="C28" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D28" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E28" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F28" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="42" t="s">
+    <row r="29" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="5">
-        <v>3</v>
-      </c>
-      <c r="D28" s="6">
-        <v>650</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F28" s="8">
-        <f>SUM(C28*D28)</f>
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="70"/>
       <c r="C29" s="5">
         <v>3</v>
       </c>
       <c r="D29" s="6">
-        <v>129</v>
+        <v>650</v>
       </c>
       <c r="E29" s="7">
         <v>0.21</v>
       </c>
       <c r="F29" s="8">
         <f>SUM(C29*D29)</f>
-        <v>387</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="43"/>
+      <c r="A30" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="70"/>
       <c r="C30" s="5">
         <v>3</v>
       </c>
       <c r="D30" s="6">
-        <v>12.9</v>
+        <v>129</v>
       </c>
       <c r="E30" s="7">
         <v>0.21</v>
       </c>
       <c r="F30" s="8">
         <f>SUM(C30*D30)</f>
-        <v>38.700000000000003</v>
+        <v>387</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="43"/>
+      <c r="A31" s="69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="70"/>
       <c r="C31" s="5">
         <v>3</v>
       </c>
       <c r="D31" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F31" s="8">
+        <f>SUM(C31*D31)</f>
+        <v>38.700000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="70"/>
+      <c r="C32" s="5">
+        <v>3</v>
+      </c>
+      <c r="D32" s="6">
         <v>9.9</v>
       </c>
-      <c r="E31" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F31" s="8">
-        <f t="shared" ref="F31:F49" si="1">SUM(C31*D31)</f>
+      <c r="E32" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" ref="F32:F52" si="1">SUM(C32*D32)</f>
         <v>29.700000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="42" t="s">
+    <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="5">
+      <c r="B33" s="70"/>
+      <c r="C33" s="5">
         <v>2</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <v>700</v>
       </c>
-      <c r="E32" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F32" s="8">
+      <c r="E33" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F33" s="8">
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="42" t="s">
+    <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="5">
+      <c r="B34" s="70"/>
+      <c r="C34" s="5">
         <v>1</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <v>375</v>
       </c>
-      <c r="E33" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="E34" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F34" s="8">
         <f t="shared" si="1"/>
         <v>375</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="43"/>
-      <c r="C34" s="5">
-        <v>1</v>
-      </c>
-      <c r="D34" s="6">
-        <v>184.9</v>
-      </c>
-      <c r="E34" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F34" s="8">
-        <f t="shared" si="1"/>
-        <v>184.9</v>
-      </c>
-    </row>
     <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="43"/>
+      <c r="A35" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="70"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
       <c r="D35" s="6">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="E35" s="7">
         <v>0.21</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="43"/>
+      <c r="A36" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="70"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
       <c r="D36" s="6">
-        <v>66.099999999999994</v>
+        <v>65</v>
       </c>
       <c r="E36" s="7">
         <v>0.21</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="1"/>
-        <v>66.099999999999994</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="43"/>
+      <c r="A37" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="70"/>
       <c r="C37" s="5">
         <v>1</v>
       </c>
       <c r="D37" s="6">
-        <v>1250</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="E37" s="7">
         <v>0.21</v>
       </c>
       <c r="F37" s="8">
         <f t="shared" si="1"/>
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="70"/>
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
         <v>1250</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="5">
-        <v>3</v>
-      </c>
-      <c r="D38" s="6">
-        <v>70</v>
       </c>
       <c r="E38" s="7">
         <v>0.21</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" si="1"/>
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="70"/>
+      <c r="C39" s="5">
+        <v>3</v>
+      </c>
+      <c r="D39" s="6">
+        <v>70</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="28" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="31">
+    <row r="40" spans="1:6" s="28" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="70"/>
+      <c r="C40" s="5">
         <v>1</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D40" s="6">
         <v>330</v>
       </c>
-      <c r="E39" s="33">
-        <v>0.21</v>
-      </c>
-      <c r="F39" s="34">
-        <f>SUM(C39*D39)</f>
+      <c r="E40" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F40" s="8">
+        <f>SUM(C40*D40)</f>
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F40" s="25"/>
-    </row>
-    <row r="41" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="25"/>
-    </row>
-    <row r="42" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="46" t="s">
+    <row r="41" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="25"/>
-    </row>
-    <row r="43" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="5">
+        <v>5</v>
+      </c>
+      <c r="D41" s="6">
+        <v>7.4</v>
+      </c>
+      <c r="E41" s="48">
+        <v>0.21</v>
+      </c>
+      <c r="F41" s="8">
+        <f>SUM(C41*D41)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="92"/>
+      <c r="C42" s="31">
+        <v>1</v>
+      </c>
+      <c r="D42" s="32">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="E42" s="49">
+        <v>0.21</v>
+      </c>
+      <c r="F42" s="34">
+        <f>SUM(C42*D42)</f>
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F43" s="25"/>
     </row>
-    <row r="44" spans="1:6" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57" t="s">
+    <row r="44" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="25"/>
+    </row>
+    <row r="45" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="91"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="25"/>
+    </row>
+    <row r="46" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" spans="1:6" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="59" t="s">
+      <c r="B47" s="90"/>
+      <c r="C47" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="59" t="s">
+      <c r="E47" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F44" s="59" t="s">
+      <c r="F47" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="49" t="s">
+    <row r="48" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="5">
+      <c r="B48" s="88"/>
+      <c r="C48" s="5">
         <v>5</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D48" s="6">
         <v>214</v>
       </c>
-      <c r="E45" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F45" s="8">
+      <c r="E48" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F48" s="8">
         <f t="shared" si="1"/>
         <v>1070</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="5">
+    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="70"/>
+      <c r="C49" s="5">
         <v>3</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D49" s="6">
         <v>126</v>
       </c>
-      <c r="E46" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F46" s="8">
+      <c r="E49" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F49" s="8">
         <f t="shared" si="1"/>
         <v>378</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="5">
-        <v>5</v>
-      </c>
-      <c r="D47" s="6">
+    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="70"/>
+      <c r="C50" s="5">
+        <v>3</v>
+      </c>
+      <c r="D50" s="6">
         <v>1755</v>
       </c>
-      <c r="E47" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F47" s="8">
+      <c r="E50" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F50" s="8">
         <f t="shared" si="1"/>
-        <v>8775</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="5">
+        <v>5265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="70"/>
+      <c r="C51" s="5">
         <v>3</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D51" s="6">
         <v>347.1</v>
       </c>
-      <c r="E48" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F48" s="8">
+      <c r="E51" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F51" s="8">
         <f t="shared" si="1"/>
         <v>1041.3000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="43"/>
-      <c r="C49" s="56">
+    <row r="52" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="70"/>
+      <c r="C52" s="43">
         <v>1</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D52" s="6">
         <v>55.78</v>
       </c>
-      <c r="E49" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="E52" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F52" s="8">
         <f t="shared" si="1"/>
         <v>55.78</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="42" t="s">
+    <row r="53" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="60"/>
-      <c r="C50" s="5">
+      <c r="B53" s="77"/>
+      <c r="C53" s="5">
         <v>5</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D53" s="6">
         <v>0</v>
       </c>
-      <c r="E50" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="E53" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F53" s="8">
         <v>0</v>
       </c>
-      <c r="G50" s="61"/>
-    </row>
-    <row r="51" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="44" t="s">
+      <c r="G53" s="44"/>
+    </row>
+    <row r="54" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="31">
+      <c r="B54" s="70"/>
+      <c r="C54" s="5">
         <v>5</v>
       </c>
-      <c r="D51" s="62">
+      <c r="D54" s="50">
         <v>0</v>
       </c>
-      <c r="E51" s="33">
-        <v>0.21</v>
-      </c>
-      <c r="F51" s="34">
-        <f>SUM(C51*D51)</f>
+      <c r="E54" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F54" s="8">
+        <f>SUM(C54*D54)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="60"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="25"/>
-    </row>
-    <row r="53" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="60"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="25"/>
-    </row>
-    <row r="54" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="60"/>
-      <c r="B54" s="60"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="25"/>
-    </row>
     <row r="55" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="60"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="25"/>
-    </row>
-    <row r="56" spans="1:7" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="60"/>
-      <c r="B56" s="60"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="25"/>
-    </row>
-    <row r="57" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-    </row>
-    <row r="58" spans="1:7" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-    </row>
-    <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D59" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="E59" s="71"/>
-      <c r="F59" s="72">
-        <f>SUM(F9:F57)</f>
-        <v>19054.859999999997</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D60" s="70" t="s">
+      <c r="A55" s="82"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="84"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="74"/>
+      <c r="B57" s="75"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="76"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="55"/>
+    </row>
+    <row r="59" spans="1:7" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="77"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="25"/>
+    </row>
+    <row r="60" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:7" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D62" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="79"/>
+      <c r="F62" s="46">
+        <f>SUM(F9:F60)</f>
+        <v>15563.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D63" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="71"/>
-      <c r="F60" s="72"/>
-    </row>
-    <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D61" s="70" t="s">
+      <c r="E63" s="79"/>
+      <c r="F63" s="46"/>
+    </row>
+    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D64" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="71"/>
-      <c r="F61" s="72">
-        <f>SUMIF(E9:E56,"=21%",F9:F56)/100*21</f>
-        <v>4001.5205999999994</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D62" s="70" t="s">
+      <c r="E64" s="79"/>
+      <c r="F64" s="46">
+        <f>SUMIF(E9:E59,"=21%",F9:F59)/100*21</f>
+        <v>3268.2321000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D65" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="71"/>
-      <c r="F62" s="72">
-        <f>SUMIF(E9:E56,"=6%",F9:F56)/100*6</f>
+      <c r="E65" s="79"/>
+      <c r="F65" s="46">
+        <f>SUMIF(E9:E59,"=6%",F9:F59)/100*6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D63" s="73" t="s">
+    <row r="66" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D66" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="74"/>
-      <c r="F63" s="75">
-        <f>SUM(F59+F61+F62-F60)</f>
-        <v>23056.380599999997</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="10"/>
-      <c r="E64" s="9"/>
-    </row>
-    <row r="66" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
-      <c r="A66" s="51" t="s">
+      <c r="E66" s="86"/>
+      <c r="F66" s="47">
+        <f>SUM(F62+F64+F65-F63)</f>
+        <v>18831.242099999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D67" s="10"/>
+      <c r="E67" s="9"/>
+    </row>
+    <row r="69" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
+      <c r="A69" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B66" s="51"/>
-      <c r="C66" s="51"/>
-      <c r="E66" s="11"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+      <c r="B69" s="64"/>
+      <c r="C69" s="64"/>
+      <c r="E69" s="11"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="4"/>
-      <c r="D71" s="17"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-    </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="39"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="40"/>
-      <c r="B75" s="40"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="40"/>
+      <c r="A74" s="4"/>
+      <c r="D74" s="17"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" s="39"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" s="40"/>
+      <c r="B78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="A66:C66"/>
+  <mergeCells count="54">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A69:C69"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.15748031496062992" top="1.75" bottom="0.74803149606299213" header="0.15748031496062992" footer="0.18"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -1991,8 +2138,8 @@
     <oddFooter>&amp;LBTW nr. BE0719379913&amp;CPagina &amp;P van &amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="23" max="5" man="1"/>
-    <brk id="40" max="16383" man="1"/>
+    <brk id="24" max="5" man="1"/>
+    <brk id="43" max="16383" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit modem + add budget config g24
</commit_message>
<xml_diff>
--- a/opdracht03/documentatie/Offerte groep 24.xlsx
+++ b/opdracht03/documentatie/Offerte groep 24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2\Vakken\Projecten 2\p2ops-g10\opdracht03\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08065E90-CAFF-4CFD-8B98-79AE9A609AB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAA77A7-C277-4976-9E7C-D4AF7CD5D75F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Offerte</t>
   </si>
@@ -198,7 +198,10 @@
     <t>Htek UC924 4-Line Gigabit - VoIP Telefoon</t>
   </si>
   <si>
-    <t>TP-Link DOCSIS 3.0 Modem</t>
+    <t>Netgear CM500-1AZNAS DOCSIS 3.0 Modem</t>
+  </si>
+  <si>
+    <t>Equip 625421 - Netwerkkabel 2 m Cat6 U/UTP</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -664,6 +667,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1085,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="11.35" x14ac:dyDescent="0.35"/>
@@ -1122,10 +1129,10 @@
       <c r="C3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="66"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
@@ -1135,15 +1142,15 @@
         <v>1001</v>
       </c>
       <c r="B4" s="36">
-        <v>43569</v>
+        <v>43575</v>
       </c>
       <c r="C4" s="37">
-        <v>43603</v>
-      </c>
-      <c r="D4" s="67" t="s">
+        <v>43605</v>
+      </c>
+      <c r="D4" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="68"/>
+      <c r="E4" s="70"/>
       <c r="F4" s="38" t="s">
         <v>11</v>
       </c>
@@ -1157,10 +1164,10 @@
       <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1175,10 +1182,10 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
@@ -1193,10 +1200,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="70"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="5">
         <v>1</v>
       </c>
@@ -1207,15 +1214,15 @@
         <v>0.21</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" ref="F9:F16" si="0">SUM(C9*D9)</f>
+        <f t="shared" ref="F9:F15" si="0">SUM(C9*D9)</f>
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="70"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="5">
         <v>1</v>
       </c>
@@ -1231,10 +1238,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="70"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="5">
         <v>1</v>
       </c>
@@ -1250,29 +1257,29 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="63" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="70"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="6">
-        <v>44.6</v>
+        <v>40.9</v>
       </c>
       <c r="E12" s="7">
         <v>0.21</v>
       </c>
       <c r="F12" s="8">
         <f>SUM(C12*D12)</f>
-        <v>44.6</v>
+        <v>40.9</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="70"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="5">
         <v>1</v>
       </c>
@@ -1288,10 +1295,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="70"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="5">
         <v>2</v>
       </c>
@@ -1307,10 +1314,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="70"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="5">
         <v>3</v>
       </c>
@@ -1326,623 +1333,635 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="72"/>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1.98</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F16" s="8">
+        <f>SUM(C16*D16)</f>
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="64" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="31">
+      <c r="B17" s="94"/>
+      <c r="C17" s="31">
         <v>5</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D17" s="32">
         <v>5.04</v>
       </c>
-      <c r="E16" s="33">
-        <v>0.21</v>
-      </c>
-      <c r="F16" s="34">
-        <f t="shared" si="0"/>
+      <c r="E17" s="49">
+        <v>0.21</v>
+      </c>
+      <c r="F17" s="65">
+        <f>SUM(C17*D17)</f>
         <v>25.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="25"/>
-    </row>
-    <row r="18" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="72"/>
+      <c r="G17" s="44"/>
+    </row>
+    <row r="18" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="30"/>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="25"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="73" t="s">
+    <row r="19" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="41" t="s">
+      <c r="B21" s="75"/>
+      <c r="C21" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D21" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E21" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F21" s="41" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="87" t="s">
+    <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="88"/>
-      <c r="C21" s="57">
+      <c r="B22" s="90"/>
+      <c r="C22" s="57">
         <v>16</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D22" s="58">
         <v>62</v>
       </c>
-      <c r="E21" s="59">
-        <v>0.21</v>
-      </c>
-      <c r="F21" s="60">
-        <f>SUM(C21*D21)</f>
+      <c r="E22" s="59">
+        <v>0.21</v>
+      </c>
+      <c r="F22" s="60">
+        <f>SUM(C22*D22)</f>
         <v>992</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="69"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="56"/>
-    </row>
     <row r="23" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="80"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="61"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="56"/>
     </row>
     <row r="24" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="71"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="25"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="61"/>
     </row>
     <row r="25" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
       <c r="C25" s="24"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
       <c r="F25" s="25"/>
     </row>
-    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="91" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
+    <row r="26" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="12"/>
       <c r="E26" s="13"/>
       <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="24"/>
+      <c r="A27" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="25"/>
     </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="73" t="s">
+    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="21" t="s">
+      <c r="B29" s="75"/>
+      <c r="C29" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E29" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F29" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="69" t="s">
+    <row r="30" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="5">
-        <v>3</v>
-      </c>
-      <c r="D29" s="6">
-        <v>650</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F29" s="8">
-        <f>SUM(C29*D29)</f>
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="70"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="5">
         <v>3</v>
       </c>
       <c r="D30" s="6">
-        <v>129</v>
+        <v>650</v>
       </c>
       <c r="E30" s="7">
         <v>0.21</v>
       </c>
       <c r="F30" s="8">
         <f>SUM(C30*D30)</f>
-        <v>387</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="70"/>
+      <c r="A31" s="71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="72"/>
       <c r="C31" s="5">
         <v>3</v>
       </c>
       <c r="D31" s="6">
-        <v>12.9</v>
+        <v>129</v>
       </c>
       <c r="E31" s="7">
         <v>0.21</v>
       </c>
       <c r="F31" s="8">
         <f>SUM(C31*D31)</f>
-        <v>38.700000000000003</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="70"/>
+      <c r="A32" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="72"/>
       <c r="C32" s="5">
         <v>3</v>
       </c>
       <c r="D32" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F32" s="8">
+        <f>SUM(C32*D32)</f>
+        <v>38.700000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="72"/>
+      <c r="C33" s="5">
+        <v>3</v>
+      </c>
+      <c r="D33" s="6">
         <v>9.9</v>
       </c>
-      <c r="E32" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F32" s="8">
-        <f t="shared" ref="F32:F52" si="1">SUM(C32*D32)</f>
+      <c r="E33" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" ref="F33:F53" si="1">SUM(C33*D33)</f>
         <v>29.700000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="69" t="s">
+    <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="70"/>
-      <c r="C33" s="5">
+      <c r="B34" s="72"/>
+      <c r="C34" s="5">
         <v>2</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <v>700</v>
       </c>
-      <c r="E33" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="E34" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F34" s="8">
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="69" t="s">
+    <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="5">
+      <c r="B35" s="72"/>
+      <c r="C35" s="5">
         <v>1</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <v>375</v>
       </c>
-      <c r="E34" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F34" s="8">
+      <c r="E35" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F35" s="8">
         <f t="shared" si="1"/>
         <v>375</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="69" t="s">
+    <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="5">
+      <c r="B36" s="72"/>
+      <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <v>119</v>
       </c>
-      <c r="E35" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="E36" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F36" s="8">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="69" t="s">
+    <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="5">
+      <c r="B37" s="72"/>
+      <c r="C37" s="5">
         <v>1</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <v>65</v>
       </c>
-      <c r="E36" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F36" s="8">
+      <c r="E37" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F37" s="8">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="69" t="s">
+    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="5">
+      <c r="B38" s="72"/>
+      <c r="C38" s="5">
         <v>1</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <v>66.099999999999994</v>
       </c>
-      <c r="E37" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F37" s="8">
+      <c r="E38" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F38" s="8">
         <f t="shared" si="1"/>
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="69" t="s">
+    <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="5">
+      <c r="B39" s="72"/>
+      <c r="C39" s="5">
         <v>1</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <v>1250</v>
       </c>
-      <c r="E38" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F38" s="8">
+      <c r="E39" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F39" s="8">
         <f t="shared" si="1"/>
         <v>1250</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="69" t="s">
+    <row r="40" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="70"/>
-      <c r="C39" s="5">
+      <c r="B40" s="72"/>
+      <c r="C40" s="5">
         <v>3</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <v>70</v>
       </c>
-      <c r="E39" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F39" s="8">
+      <c r="E40" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F40" s="8">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="28" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="69" t="s">
+    <row r="41" spans="1:6" s="28" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="70"/>
-      <c r="C40" s="5">
+      <c r="B41" s="72"/>
+      <c r="C41" s="5">
         <v>1</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <v>330</v>
       </c>
-      <c r="E40" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F40" s="8">
-        <f>SUM(C40*D40)</f>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="77"/>
-      <c r="C41" s="5">
-        <v>5</v>
-      </c>
-      <c r="D41" s="6">
-        <v>7.4</v>
-      </c>
-      <c r="E41" s="48">
+      <c r="E41" s="7">
         <v>0.21</v>
       </c>
       <c r="F41" s="8">
         <f>SUM(C41*D41)</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="79"/>
+      <c r="C42" s="5">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6">
+        <v>7.4</v>
+      </c>
+      <c r="E42" s="48">
+        <v>0.21</v>
+      </c>
+      <c r="F42" s="8">
+        <f>SUM(C42*D42)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="80" t="s">
+    <row r="43" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="92"/>
-      <c r="C42" s="31">
+      <c r="B43" s="94"/>
+      <c r="C43" s="31">
         <v>1</v>
       </c>
-      <c r="D42" s="32">
+      <c r="D43" s="32">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E42" s="49">
-        <v>0.21</v>
-      </c>
-      <c r="F42" s="34">
-        <f>SUM(C42*D42)</f>
+      <c r="E43" s="49">
+        <v>0.21</v>
+      </c>
+      <c r="F43" s="34">
+        <f>SUM(C43*D43)</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F43" s="25"/>
-    </row>
-    <row r="44" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
+    <row r="44" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F44" s="25"/>
     </row>
-    <row r="45" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="91"/>
+    <row r="45" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="30"/>
       <c r="D45" s="12"/>
       <c r="E45" s="13"/>
       <c r="F45" s="25"/>
     </row>
     <row r="46" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
+      <c r="A46" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="93"/>
       <c r="C46" s="30"/>
       <c r="D46" s="12"/>
       <c r="E46" s="13"/>
       <c r="F46" s="25"/>
     </row>
-    <row r="47" spans="1:6" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="89" t="s">
+    <row r="47" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="1:6" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="90"/>
-      <c r="C47" s="21" t="s">
+      <c r="B48" s="92"/>
+      <c r="C48" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="D48" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E48" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F48" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="87" t="s">
+    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="88"/>
-      <c r="C48" s="5">
+      <c r="B49" s="90"/>
+      <c r="C49" s="5">
         <v>5</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <v>214</v>
       </c>
-      <c r="E48" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F48" s="8">
+      <c r="E49" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F49" s="8">
         <f t="shared" si="1"/>
         <v>1070</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="69" t="s">
+    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="70"/>
-      <c r="C49" s="5">
+      <c r="B50" s="72"/>
+      <c r="C50" s="5">
         <v>3</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <v>126</v>
       </c>
-      <c r="E49" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="E50" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F50" s="8">
         <f t="shared" si="1"/>
         <v>378</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="69" t="s">
+    <row r="51" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="70"/>
-      <c r="C50" s="5">
+      <c r="B51" s="72"/>
+      <c r="C51" s="5">
         <v>3</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <v>1755</v>
       </c>
-      <c r="E50" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="E51" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F51" s="8">
         <f t="shared" si="1"/>
         <v>5265</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="69" t="s">
+    <row r="52" spans="1:7" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="70"/>
-      <c r="C51" s="5">
+      <c r="B52" s="72"/>
+      <c r="C52" s="5">
         <v>3</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <v>347.1</v>
       </c>
-      <c r="E51" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F51" s="8">
+      <c r="E52" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F52" s="8">
         <f t="shared" si="1"/>
         <v>1041.3000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="69" t="s">
+    <row r="53" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="70"/>
-      <c r="C52" s="43">
+      <c r="B53" s="72"/>
+      <c r="C53" s="43">
         <v>1</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <v>55.78</v>
       </c>
-      <c r="E52" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F52" s="8">
+      <c r="E53" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F53" s="8">
         <f t="shared" si="1"/>
         <v>55.78</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="69" t="s">
+    <row r="54" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="5">
-        <v>5</v>
-      </c>
-      <c r="D53" s="6">
-        <v>0</v>
-      </c>
-      <c r="E53" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F53" s="8">
-        <v>0</v>
-      </c>
-      <c r="G53" s="44"/>
-    </row>
-    <row r="54" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="70"/>
+      <c r="B54" s="79"/>
       <c r="C54" s="5">
         <v>5</v>
       </c>
-      <c r="D54" s="50">
+      <c r="D54" s="6">
         <v>0</v>
       </c>
       <c r="E54" s="7">
         <v>0.21</v>
       </c>
       <c r="F54" s="8">
-        <f>SUM(C54*D54)</f>
         <v>0</v>
       </c>
+      <c r="G54" s="44"/>
     </row>
     <row r="55" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="82"/>
-      <c r="B55" s="83"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="8"/>
+      <c r="A55" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="72"/>
+      <c r="C55" s="5">
+        <v>5</v>
+      </c>
+      <c r="D55" s="50">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F55" s="8">
+        <f>SUM(C55*D55)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="84"/>
-      <c r="B56" s="83"/>
+      <c r="B56" s="85"/>
       <c r="C56" s="51"/>
       <c r="D56" s="50"/>
       <c r="E56" s="7"/>
       <c r="F56" s="8"/>
     </row>
     <row r="57" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="74"/>
-      <c r="B57" s="75"/>
+      <c r="A57" s="86"/>
+      <c r="B57" s="85"/>
       <c r="C57" s="51"/>
       <c r="D57" s="50"/>
       <c r="E57" s="7"/>
@@ -1950,29 +1969,29 @@
     </row>
     <row r="58" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="76"/>
-      <c r="B58" s="76"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="55"/>
-    </row>
-    <row r="59" spans="1:7" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="77"/>
-      <c r="B59" s="77"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="25"/>
-    </row>
-    <row r="60" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-    </row>
-    <row r="61" spans="1:7" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="77"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="78"/>
+      <c r="B59" s="78"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="55"/>
+    </row>
+    <row r="60" spans="1:7" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="79"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="25"/>
+    </row>
+    <row r="61" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1980,152 +1999,161 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D62" s="78" t="s">
+    <row r="62" spans="1:7" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D63" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="E62" s="79"/>
-      <c r="F62" s="46">
-        <f>SUM(F9:F60)</f>
-        <v>15563.01</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D63" s="78" t="s">
+      <c r="E63" s="81"/>
+      <c r="F63" s="46">
+        <f>SUM(F9:F61)</f>
+        <v>15561.289999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D64" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="79"/>
-      <c r="F63" s="46"/>
-    </row>
-    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="78" t="s">
+      <c r="E64" s="81"/>
+      <c r="F64" s="46"/>
+    </row>
+    <row r="65" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D65" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="E64" s="79"/>
-      <c r="F64" s="46">
-        <f>SUMIF(E9:E59,"=21%",F9:F59)/100*21</f>
-        <v>3268.2321000000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D65" s="78" t="s">
+      <c r="E65" s="81"/>
+      <c r="F65" s="46">
+        <f>SUMIF(E9:E60,"=21%",F9:F60)/100*21</f>
+        <v>3267.8708999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D66" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="79"/>
-      <c r="F65" s="46">
-        <f>SUMIF(E9:E59,"=6%",F9:F59)/100*6</f>
+      <c r="E66" s="81"/>
+      <c r="F66" s="46">
+        <f>SUMIF(E9:E60,"=6%",F9:F60)/100*6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D66" s="85" t="s">
+    <row r="67" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D67" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="86"/>
-      <c r="F66" s="47">
-        <f>SUM(F62+F64+F65-F63)</f>
-        <v>18831.242099999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D67" s="10"/>
-      <c r="E67" s="9"/>
-    </row>
-    <row r="69" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
-      <c r="A69" s="64" t="s">
+      <c r="E67" s="88"/>
+      <c r="F67" s="47">
+        <f>SUM(F63+F65+F66-F64)</f>
+        <v>18829.160899999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="D68" s="10"/>
+      <c r="E68" s="9"/>
+    </row>
+    <row r="70" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
+      <c r="A70" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="E69" s="11"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
+      <c r="B70" s="66"/>
+      <c r="C70" s="66"/>
+      <c r="E70" s="11"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="4"/>
-      <c r="D74" s="17"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="4"/>
+      <c r="D75" s="17"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="39"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
       <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="40"/>
-      <c r="B78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
+      <c r="A78" s="39"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" s="40"/>
+      <c r="B79" s="40"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="55">
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A70:C70"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.15748031496062992" top="1.75" bottom="0.74803149606299213" header="0.15748031496062992" footer="0.18"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
@@ -2138,8 +2166,8 @@
     <oddFooter>&amp;LBTW nr. BE0719379913&amp;CPagina &amp;P van &amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="24" max="5" man="1"/>
-    <brk id="43" max="16383" man="1"/>
+    <brk id="25" max="5" man="1"/>
+    <brk id="44" max="16383" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
G24-36-40 Offertes + Voorstelling
</commit_message>
<xml_diff>
--- a/opdracht03/documentatie/Offerte groep 24.xlsx
+++ b/opdracht03/documentatie/Offerte groep 24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2\Vakken\Projecten 2\p2ops-g10\opdracht03\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAA77A7-C277-4976-9E7C-D4AF7CD5D75F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8F64C7-B88D-4FA2-8C2D-485F7355EE03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Offerte</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Subtotaal</t>
   </si>
   <si>
-    <t>Korting</t>
-  </si>
-  <si>
     <t>BTW bedrag 6%</t>
   </si>
   <si>
@@ -195,13 +192,19 @@
     <t>Microsoft Office 365 Business Premium - 1 jaar</t>
   </si>
   <si>
-    <t>Htek UC924 4-Line Gigabit - VoIP Telefoon</t>
-  </si>
-  <si>
     <t>Netgear CM500-1AZNAS DOCSIS 3.0 Modem</t>
   </si>
   <si>
     <t>Equip 625421 - Netwerkkabel 2 m Cat6 U/UTP</t>
+  </si>
+  <si>
+    <t>Installatie &amp; Opleiding</t>
+  </si>
+  <si>
+    <t>VoIP huur toestel - 1 jaar</t>
+  </si>
+  <si>
+    <t>VoIP Telenet FreePhone Business abonnement per gebruiker - 1 jaar</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -671,6 +674,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1094,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="11.35" x14ac:dyDescent="0.35"/>
@@ -1127,12 +1131,12 @@
         <v>2</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="68"/>
+        <v>9</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="69"/>
       <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
@@ -1147,12 +1151,12 @@
       <c r="C4" s="37">
         <v>43605</v>
       </c>
-      <c r="D4" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="70"/>
+      <c r="D4" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="71"/>
       <c r="F4" s="38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.35" x14ac:dyDescent="0.5">
@@ -1164,10 +1168,10 @@
       <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="74" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="74"/>
+      <c r="A6" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="75"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1182,15 +1186,15 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="76"/>
+      <c r="C8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>13</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>4</v>
@@ -1200,10 +1204,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="71" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="72"/>
+      <c r="A9" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="73"/>
       <c r="C9" s="5">
         <v>1</v>
       </c>
@@ -1219,10 +1223,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="72"/>
+      <c r="A10" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="73"/>
       <c r="C10" s="5">
         <v>1</v>
       </c>
@@ -1238,10 +1242,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="72"/>
+      <c r="A11" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="73"/>
       <c r="C11" s="5">
         <v>1</v>
       </c>
@@ -1257,10 +1261,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" s="63" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="72"/>
+      <c r="A12" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="73"/>
       <c r="C12" s="5">
         <v>1</v>
       </c>
@@ -1276,10 +1280,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="72"/>
+      <c r="A13" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="73"/>
       <c r="C13" s="5">
         <v>1</v>
       </c>
@@ -1295,10 +1299,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="72"/>
+      <c r="A14" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="73"/>
       <c r="C14" s="5">
         <v>2</v>
       </c>
@@ -1314,10 +1318,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="72"/>
+      <c r="A15" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="73"/>
       <c r="C15" s="5">
         <v>3</v>
       </c>
@@ -1333,10 +1337,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="72"/>
+      <c r="A16" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="73"/>
       <c r="C16" s="5">
         <v>1</v>
       </c>
@@ -1352,10 +1356,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="64" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="94"/>
+      <c r="A17" s="83" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="95"/>
       <c r="C17" s="31">
         <v>5</v>
       </c>
@@ -1380,10 +1384,10 @@
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="74"/>
+      <c r="A19" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="75"/>
       <c r="C19" s="30"/>
       <c r="D19" s="12"/>
       <c r="E19" s="13"/>
@@ -1401,15 +1405,15 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="75"/>
+      <c r="A21" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="76"/>
       <c r="C21" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="41" t="s">
         <v>40</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>41</v>
       </c>
       <c r="E21" s="41" t="s">
         <v>4</v>
@@ -1419,12 +1423,12 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="89" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="90"/>
+      <c r="A22" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="91"/>
       <c r="C22" s="57">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D22" s="58">
         <v>62</v>
@@ -1434,28 +1438,28 @@
       </c>
       <c r="F22" s="60">
         <f>SUM(C22*D22)</f>
-        <v>992</v>
+        <v>3472</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="51"/>
       <c r="D23" s="50"/>
       <c r="E23" s="7"/>
       <c r="F23" s="56"/>
     </row>
     <row r="24" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="82"/>
-      <c r="B24" s="83"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="62"/>
       <c r="D24" s="45"/>
       <c r="E24" s="33"/>
       <c r="F24" s="61"/>
     </row>
     <row r="25" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="24"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
@@ -1470,11 +1474,11 @@
       <c r="F26" s="25"/>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="93" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="93"/>
+      <c r="A27" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="25"/>
@@ -1488,15 +1492,15 @@
       <c r="F28" s="25"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="76"/>
+      <c r="C29" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>12</v>
-      </c>
-      <c r="B29" s="75"/>
-      <c r="C29" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>13</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>4</v>
@@ -1506,10 +1510,10 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="71" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="72"/>
+      <c r="A30" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="73"/>
       <c r="C30" s="5">
         <v>3</v>
       </c>
@@ -1525,10 +1529,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="72"/>
+      <c r="A31" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="73"/>
       <c r="C31" s="5">
         <v>3</v>
       </c>
@@ -1544,10 +1548,10 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="71" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="72"/>
+      <c r="A32" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="73"/>
       <c r="C32" s="5">
         <v>3</v>
       </c>
@@ -1563,10 +1567,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="71" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="72"/>
+      <c r="A33" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="73"/>
       <c r="C33" s="5">
         <v>3</v>
       </c>
@@ -1577,15 +1581,15 @@
         <v>0.21</v>
       </c>
       <c r="F33" s="8">
-        <f t="shared" ref="F33:F53" si="1">SUM(C33*D33)</f>
+        <f t="shared" ref="F33:F54" si="1">SUM(C33*D33)</f>
         <v>29.700000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="72"/>
+      <c r="A34" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="73"/>
       <c r="C34" s="5">
         <v>2</v>
       </c>
@@ -1601,10 +1605,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="72"/>
+      <c r="A35" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="73"/>
       <c r="C35" s="5">
         <v>1</v>
       </c>
@@ -1620,10 +1624,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="72"/>
+      <c r="A36" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="73"/>
       <c r="C36" s="5">
         <v>1</v>
       </c>
@@ -1639,10 +1643,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="72"/>
+      <c r="A37" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="73"/>
       <c r="C37" s="5">
         <v>1</v>
       </c>
@@ -1658,10 +1662,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="72"/>
+      <c r="A38" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="73"/>
       <c r="C38" s="5">
         <v>1</v>
       </c>
@@ -1677,10 +1681,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="71" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="72"/>
+      <c r="A39" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="73"/>
       <c r="C39" s="5">
         <v>1</v>
       </c>
@@ -1695,311 +1699,322 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="72"/>
+    <row r="40" spans="1:6" s="66" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="73"/>
       <c r="C40" s="5">
         <v>3</v>
       </c>
       <c r="D40" s="6">
-        <v>70</v>
+        <v>198</v>
       </c>
       <c r="E40" s="7">
         <v>0.21</v>
       </c>
       <c r="F40" s="8">
         <f t="shared" si="1"/>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="28" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="72"/>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="73"/>
       <c r="C41" s="5">
+        <v>3</v>
+      </c>
+      <c r="D41" s="6">
+        <v>49.5</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="1"/>
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="28" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="73"/>
+      <c r="C42" s="5">
         <v>1</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <v>330</v>
       </c>
-      <c r="E41" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F41" s="8">
-        <f>SUM(C41*D41)</f>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="79"/>
-      <c r="C42" s="5">
-        <v>5</v>
-      </c>
-      <c r="D42" s="6">
-        <v>7.4</v>
-      </c>
-      <c r="E42" s="48">
+      <c r="E42" s="7">
         <v>0.21</v>
       </c>
       <c r="F42" s="8">
         <f>SUM(C42*D42)</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="80"/>
+      <c r="C43" s="5">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6">
+        <v>7.4</v>
+      </c>
+      <c r="E43" s="48">
+        <v>0.21</v>
+      </c>
+      <c r="F43" s="8">
+        <f>SUM(C43*D43)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="82" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="94"/>
-      <c r="C43" s="31">
+    <row r="44" spans="1:6" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="95"/>
+      <c r="C44" s="31">
         <v>1</v>
       </c>
-      <c r="D43" s="32">
+      <c r="D44" s="32">
         <v>2.4500000000000002</v>
       </c>
-      <c r="E43" s="49">
-        <v>0.21</v>
-      </c>
-      <c r="F43" s="34">
-        <f>SUM(C43*D43)</f>
+      <c r="E44" s="49">
+        <v>0.21</v>
+      </c>
+      <c r="F44" s="34">
+        <f>SUM(C44*D44)</f>
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F44" s="25"/>
-    </row>
-    <row r="45" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
+    <row r="45" spans="1:6" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F45" s="25"/>
     </row>
-    <row r="46" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="93" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="93"/>
+    <row r="46" spans="1:6" s="28" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="30"/>
       <c r="D46" s="12"/>
       <c r="E46" s="13"/>
       <c r="F46" s="25"/>
     </row>
     <row r="47" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
+      <c r="A47" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="94"/>
       <c r="C47" s="30"/>
       <c r="D47" s="12"/>
       <c r="E47" s="13"/>
       <c r="F47" s="25"/>
     </row>
-    <row r="48" spans="1:6" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="91" t="s">
+    <row r="48" spans="1:6" s="28" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="25"/>
+    </row>
+    <row r="49" spans="1:7" s="28" customFormat="1" ht="15.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="92" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="93"/>
+      <c r="C49" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="92"/>
-      <c r="C48" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="21" t="s">
+      <c r="E49" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="F49" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" s="90"/>
-      <c r="C49" s="5">
+    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="91"/>
+      <c r="C50" s="5">
         <v>5</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <v>214</v>
       </c>
-      <c r="E49" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="E50" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F50" s="8">
         <f t="shared" si="1"/>
         <v>1070</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="72"/>
-      <c r="C50" s="5">
+    <row r="51" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="73"/>
+      <c r="C51" s="5">
         <v>3</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <v>126</v>
       </c>
-      <c r="E50" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="E51" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F51" s="8">
         <f t="shared" si="1"/>
         <v>378</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="B51" s="72"/>
-      <c r="C51" s="5">
+    <row r="52" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="73"/>
+      <c r="C52" s="5">
         <v>3</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <v>1755</v>
       </c>
-      <c r="E51" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F51" s="8">
+      <c r="E52" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F52" s="8">
         <f t="shared" si="1"/>
         <v>5265</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="72"/>
-      <c r="C52" s="5">
+    <row r="53" spans="1:7" s="27" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="73"/>
+      <c r="C53" s="5">
         <v>3</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <v>347.1</v>
       </c>
-      <c r="E52" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F52" s="8">
+      <c r="E53" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F53" s="8">
         <f t="shared" si="1"/>
         <v>1041.3000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="72"/>
-      <c r="C53" s="43">
+    <row r="54" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="73"/>
+      <c r="C54" s="43">
         <v>1</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <v>55.78</v>
       </c>
-      <c r="E53" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F53" s="8">
+      <c r="E54" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F54" s="8">
         <f t="shared" si="1"/>
         <v>55.78</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="71" t="s">
-        <v>20</v>
-      </c>
-      <c r="B54" s="79"/>
-      <c r="C54" s="5">
-        <v>5</v>
-      </c>
-      <c r="D54" s="6">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7">
-        <v>0.21</v>
-      </c>
-      <c r="F54" s="8">
-        <v>0</v>
-      </c>
-      <c r="G54" s="44"/>
-    </row>
     <row r="55" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B55" s="72"/>
+      <c r="B55" s="80"/>
       <c r="C55" s="5">
         <v>5</v>
       </c>
-      <c r="D55" s="50">
+      <c r="D55" s="6">
         <v>0</v>
       </c>
       <c r="E55" s="7">
         <v>0.21</v>
       </c>
       <c r="F55" s="8">
-        <f>SUM(C55*D55)</f>
         <v>0</v>
       </c>
+      <c r="G55" s="44"/>
     </row>
     <row r="56" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="84"/>
-      <c r="B56" s="85"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="8"/>
+      <c r="A56" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="73"/>
+      <c r="C56" s="5">
+        <v>5</v>
+      </c>
+      <c r="D56" s="50">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="F56" s="8">
+        <f>SUM(C56*D56)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="86"/>
-      <c r="B57" s="85"/>
+      <c r="A57" s="85"/>
+      <c r="B57" s="86"/>
       <c r="C57" s="51"/>
       <c r="D57" s="50"/>
       <c r="E57" s="7"/>
       <c r="F57" s="8"/>
     </row>
     <row r="58" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="76"/>
-      <c r="B58" s="77"/>
+      <c r="A58" s="87"/>
+      <c r="B58" s="86"/>
       <c r="C58" s="51"/>
       <c r="D58" s="50"/>
       <c r="E58" s="7"/>
       <c r="F58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="78"/>
+      <c r="A59" s="77"/>
       <c r="B59" s="78"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="55"/>
-    </row>
-    <row r="60" spans="1:7" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C59" s="51"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="79"/>
       <c r="B60" s="79"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="25"/>
-    </row>
-    <row r="61" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="1:7" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C60" s="52"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="55"/>
+    </row>
+    <row r="61" spans="1:7" ht="37.35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="80"/>
+      <c r="B61" s="80"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="25"/>
+    </row>
+    <row r="62" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2007,51 +2022,52 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D63" s="80" t="s">
-        <v>46</v>
-      </c>
-      <c r="E63" s="81"/>
-      <c r="F63" s="46">
-        <f>SUM(F9:F61)</f>
-        <v>15561.289999999999</v>
-      </c>
+    <row r="63" spans="1:7" s="27" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="80" t="s">
+      <c r="D64" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="E64" s="82"/>
+      <c r="F64" s="46">
+        <f>SUM(F9:F62)</f>
+        <v>18573.789999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D65" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="82"/>
+      <c r="F65" s="46">
+        <f>SUMIF(E9:E61,"=21%",F9:F61)/100*21</f>
+        <v>3900.4958999999994</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D66" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="81"/>
-      <c r="F64" s="46"/>
-    </row>
-    <row r="65" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D65" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="81"/>
-      <c r="F65" s="46">
-        <f>SUMIF(E9:E60,"=21%",F9:F60)/100*21</f>
-        <v>3267.8708999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D66" s="80" t="s">
+      <c r="E66" s="82"/>
+      <c r="F66" s="46">
+        <f>SUMIF(E9:E61,"=6%",F9:F61)/100*6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D67" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="81"/>
-      <c r="F66" s="46">
-        <f>SUMIF(E9:E60,"=6%",F9:F60)/100*6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D67" s="87" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="88"/>
+      <c r="E67" s="89"/>
       <c r="F67" s="47">
-        <f>SUM(F63+F65+F66-F64)</f>
-        <v>18829.160899999999</v>
+        <f>SUM(F64+F65+F66)</f>
+        <v>22474.285899999995</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="11.7" thickTop="1" x14ac:dyDescent="0.35">
@@ -2059,19 +2075,19 @@
       <c r="E68" s="9"/>
     </row>
     <row r="70" spans="1:6" ht="11.7" x14ac:dyDescent="0.4">
-      <c r="A70" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70" s="66"/>
-      <c r="C70" s="66"/>
+      <c r="A70" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="67"/>
+      <c r="C70" s="67"/>
       <c r="E70" s="11"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -2101,19 +2117,20 @@
   <mergeCells count="55">
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A47:B47"/>
     <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A40:B40"/>
     <mergeCell ref="D66:E66"/>
     <mergeCell ref="D67:E67"/>
     <mergeCell ref="A13:B13"/>
@@ -2126,18 +2143,17 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A51:B51"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A53:B53"/>
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -2147,10 +2163,10 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D64:E64"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A30:B30"/>
@@ -2167,7 +2183,7 @@
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="25" max="5" man="1"/>
-    <brk id="44" max="16383" man="1"/>
+    <brk id="45" max="16383" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>